<commit_message>
change practice to calibration trials
</commit_message>
<xml_diff>
--- a/pract1.xlsx
+++ b/pract1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alisaloosen/Documents/GitHub/RewardEffortLearningTask/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB87911-7A4B-354F-8100-CFE343B1999D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508C50CB-87FF-0044-A866-DE21CF35C956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{173F3EE6-8704-894A-AAEC-171090EC6741}"/>
   </bookViews>
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB1A174-335D-084B-A5B3-FF71FE9BFFA4}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -433,6 +433,14 @@
         <v>-0.09</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>100</v>
+      </c>
+      <c r="B5">
+        <v>0.05</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>